<commit_message>
sửa Tạo TT Khách hàng thành cập nhật thông tin khách hàng
</commit_message>
<xml_diff>
--- a/barchartQLKDBH.xlsx
+++ b/barchartQLKDBH.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70412D8D-391A-4A78-BBE2-AFC090AB1F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D807EB-7C53-4C1B-8D77-509AB7C05403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2880" windowWidth="21600" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
   <si>
     <t>Project Start:</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Tìm kiếm thông tin khách hàng</t>
   </si>
   <si>
-    <t>Tạo thông tin khách hàng</t>
-  </si>
-  <si>
     <t>Tạo thông tin nhân viên</t>
   </si>
   <si>
@@ -355,6 +352,12 @@
   </si>
   <si>
     <t>In phiếu thanh toán nợ</t>
+  </si>
+  <si>
+    <t>Xem danh sách nhân viên</t>
+  </si>
+  <si>
+    <t>Cập nhật thông tin khách hàng</t>
   </si>
 </sst>
 </file>
@@ -2634,11 +2637,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL59"/>
+  <dimension ref="A1:BL60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="6" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2689,7 +2692,7 @@
       <c r="D3" s="92"/>
       <c r="E3" s="97">
         <f ca="1">TODAY()</f>
-        <v>44144</v>
+        <v>44147</v>
       </c>
       <c r="F3" s="97"/>
     </row>
@@ -3351,7 +3354,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
-        <f t="shared" ref="H8:H46" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H47" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="35"/>
@@ -3426,11 +3429,11 @@
       </c>
       <c r="E9" s="55">
         <f ca="1">Project_Start</f>
-        <v>44144</v>
+        <v>44147</v>
       </c>
       <c r="F9" s="55">
         <f ca="1">E9+3</f>
-        <v>44147</v>
+        <v>44150</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14">
@@ -3509,11 +3512,11 @@
       </c>
       <c r="E10" s="55">
         <f ca="1">F9</f>
-        <v>44147</v>
+        <v>44150</v>
       </c>
       <c r="F10" s="55">
         <f ca="1">E10+2</f>
-        <v>44149</v>
+        <v>44152</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14">
@@ -3590,11 +3593,11 @@
       </c>
       <c r="E11" s="55">
         <f ca="1">F10</f>
-        <v>44149</v>
+        <v>44152</v>
       </c>
       <c r="F11" s="55">
         <f ca="1">E11+4</f>
-        <v>44153</v>
+        <v>44156</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14">
@@ -3895,7 +3898,7 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49"/>
       <c r="B15" s="73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="62" t="s">
         <v>57</v>
@@ -3976,7 +3979,7 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49"/>
       <c r="B16" s="73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>57</v>
@@ -4209,7 +4212,7 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="48"/>
       <c r="B19" s="74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>58</v>
@@ -4300,11 +4303,11 @@
       </c>
       <c r="E20" s="57">
         <f ca="1">E9+15</f>
-        <v>44159</v>
+        <v>44162</v>
       </c>
       <c r="F20" s="57">
         <f ca="1">E20+5</f>
-        <v>44164</v>
+        <v>44167</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14">
@@ -4371,7 +4374,7 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="48"/>
       <c r="B21" s="74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="64" t="s">
         <v>58</v>
@@ -4381,11 +4384,11 @@
       </c>
       <c r="E21" s="57">
         <f ca="1">E10+15</f>
-        <v>44162</v>
+        <v>44165</v>
       </c>
       <c r="F21" s="57">
         <f ca="1">E21+5</f>
-        <v>44167</v>
+        <v>44170</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14">
@@ -4533,7 +4536,7 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="48"/>
       <c r="B23" s="74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="64" t="s">
         <v>57</v>
@@ -4543,11 +4546,11 @@
       </c>
       <c r="E23" s="57">
         <f ca="1">F20+1</f>
-        <v>44165</v>
+        <v>44168</v>
       </c>
       <c r="F23" s="57">
         <f ca="1">E23+4</f>
-        <v>44169</v>
+        <v>44172</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14">
@@ -4766,7 +4769,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="66" t="s">
         <v>58</v>
@@ -4845,7 +4848,7 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="48"/>
       <c r="B27" s="75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="66" t="s">
         <v>57</v>
@@ -4924,7 +4927,7 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="48"/>
       <c r="B28" s="75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="66" t="s">
         <v>57</v>
@@ -5155,7 +5158,7 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48"/>
       <c r="B31" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="66" t="s">
         <v>57</v>
@@ -5236,11 +5239,9 @@
         <v>24</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>56</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C32" s="66"/>
       <c r="D32" s="34">
         <v>0.5</v>
       </c>
@@ -5251,10 +5252,7 @@
         <v>44141</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="14">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
+      <c r="H32" s="14"/>
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
@@ -5315,24 +5313,24 @@
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="48"/>
       <c r="B33" s="75" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="34">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="58">
-        <v>44131</v>
+        <v>44138</v>
       </c>
       <c r="F33" s="58">
-        <v>44133</v>
+        <v>44141</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
@@ -5394,7 +5392,7 @@
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="48"/>
       <c r="B34" s="75" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C34" s="66" t="s">
         <v>57</v>
@@ -5473,24 +5471,24 @@
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="B35" s="75" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D35" s="34">
         <v>0.25</v>
       </c>
       <c r="E35" s="58">
-        <v>44134</v>
+        <v>44131</v>
       </c>
       <c r="F35" s="58">
-        <v>44137</v>
+        <v>44133</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>3</v>
       </c>
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
@@ -5552,7 +5550,7 @@
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48"/>
       <c r="B36" s="75" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="66" t="s">
         <v>55</v>
@@ -5630,17 +5628,25 @@
     </row>
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48"/>
-      <c r="B37" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="81"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="84"/>
+      <c r="B37" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="E37" s="58">
+        <v>44134</v>
+      </c>
+      <c r="F37" s="58">
+        <v>44137</v>
+      </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="14" t="str">
+      <c r="H37" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
@@ -5703,25 +5709,17 @@
       <c r="A38" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="75" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="E38" s="58">
-        <v>44138</v>
-      </c>
-      <c r="F38" s="58">
-        <v>44141</v>
-      </c>
+      <c r="B38" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="81"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="84"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="14">
+      <c r="H38" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I38" s="35"/>
       <c r="J38" s="35"/>
@@ -5785,24 +5783,24 @@
         <v>25</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C39" s="66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" s="34">
-        <v>0.55000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="E39" s="58">
-        <v>44142</v>
+        <v>44138</v>
       </c>
       <c r="F39" s="58">
-        <v>44146</v>
+        <v>44141</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="14">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -5863,7 +5861,7 @@
     </row>
     <row r="40" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="75" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C40" s="66" t="s">
         <v>58</v>
@@ -5940,17 +5938,25 @@
       <c r="BL40" s="35"/>
     </row>
     <row r="41" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="85" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="86"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="88"/>
-      <c r="F41" s="89"/>
+      <c r="B41" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="34">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E41" s="58">
+        <v>44142</v>
+      </c>
+      <c r="F41" s="58">
+        <v>44146</v>
+      </c>
       <c r="G41" s="14"/>
-      <c r="H41" s="14" t="str">
+      <c r="H41" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
@@ -6010,25 +6016,17 @@
       <c r="BL41" s="35"/>
     </row>
     <row r="42" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="34">
-        <v>1</v>
-      </c>
-      <c r="E42" s="58">
-        <v>44148</v>
-      </c>
-      <c r="F42" s="58">
-        <v>44150</v>
-      </c>
+      <c r="B42" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="86"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="89"/>
       <c r="G42" s="14"/>
-      <c r="H42" s="14">
+      <c r="H42" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
@@ -6089,24 +6087,24 @@
     </row>
     <row r="43" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="75" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C43" s="66" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D43" s="34">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="E43" s="58">
         <v>44148</v>
       </c>
       <c r="F43" s="58">
-        <v>44151</v>
+        <v>44150</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="14">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I43" s="35"/>
       <c r="J43" s="35"/>
@@ -6167,19 +6165,19 @@
     </row>
     <row r="44" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="75" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C44" s="66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" s="34">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="E44" s="58">
-        <v>44152</v>
+        <v>44148</v>
       </c>
       <c r="F44" s="58">
-        <v>44155</v>
+        <v>44151</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14">
@@ -6244,17 +6242,25 @@
       <c r="BL44" s="35"/>
     </row>
     <row r="45" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="68"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71"/>
+      <c r="B45" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="58">
+        <v>44152</v>
+      </c>
+      <c r="F45" s="58">
+        <v>44155</v>
+      </c>
       <c r="G45" s="14"/>
-      <c r="H45" s="14" t="str">
+      <c r="H45" s="14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="I45" s="35"/>
       <c r="J45" s="35"/>
@@ -6314,25 +6320,17 @@
       <c r="BL45" s="35"/>
     </row>
     <row r="46" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="34">
-        <v>0.35</v>
-      </c>
-      <c r="E46" s="58">
-        <v>44156</v>
-      </c>
-      <c r="F46" s="58">
-        <v>44159</v>
-      </c>
+      <c r="B46" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="71"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="14">
+      <c r="H46" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I46" s="35"/>
       <c r="J46" s="35"/>
@@ -6393,14 +6391,25 @@
     </row>
     <row r="47" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
+        <v>95</v>
+      </c>
+      <c r="C47" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="34">
+        <v>0.35</v>
+      </c>
+      <c r="E47" s="58">
+        <v>44156</v>
+      </c>
+      <c r="F47" s="58">
+        <v>44159</v>
+      </c>
       <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="H47" s="14">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
       <c r="I47" s="35"/>
       <c r="J47" s="35"/>
       <c r="K47" s="35"/>
@@ -6460,7 +6469,7 @@
     </row>
     <row r="48" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="75" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C48" s="66"/>
       <c r="D48" s="34"/>
@@ -6527,7 +6536,7 @@
     </row>
     <row r="49" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="75" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C49" s="66"/>
       <c r="D49" s="34"/>
@@ -6593,18 +6602,15 @@
       <c r="BL49" s="35"/>
     </row>
     <row r="50" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="68"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="71"/>
+      <c r="B50" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="66"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="14" t="str">
-        <f t="shared" ref="H50:H51" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
+      <c r="H50" s="14"/>
       <c r="I50" s="35"/>
       <c r="J50" s="35"/>
       <c r="K50" s="35"/>
@@ -6663,25 +6669,17 @@
       <c r="BL50" s="35"/>
     </row>
     <row r="51" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="34">
-        <v>0.35</v>
-      </c>
-      <c r="E51" s="58">
-        <v>44156</v>
-      </c>
-      <c r="F51" s="58">
-        <v>44159</v>
-      </c>
+      <c r="B51" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="68"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="71"/>
       <c r="G51" s="14"/>
-      <c r="H51" s="14">
-        <f t="shared" si="7"/>
-        <v>4</v>
+      <c r="H51" s="14" t="str">
+        <f t="shared" ref="H51:H52" si="7">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
       </c>
       <c r="I51" s="35"/>
       <c r="J51" s="35"/>
@@ -6742,14 +6740,25 @@
     </row>
     <row r="52" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="75" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="66"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
+        <v>84</v>
+      </c>
+      <c r="C52" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="34">
+        <v>0.35</v>
+      </c>
+      <c r="E52" s="58">
+        <v>44156</v>
+      </c>
+      <c r="F52" s="58">
+        <v>44159</v>
+      </c>
       <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
+      <c r="H52" s="14">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
       <c r="I52" s="35"/>
       <c r="J52" s="35"/>
       <c r="K52" s="35"/>
@@ -6809,7 +6818,7 @@
     </row>
     <row r="53" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="75" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C53" s="66"/>
       <c r="D53" s="34"/>
@@ -6876,7 +6885,7 @@
     </row>
     <row r="54" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C54" s="66"/>
       <c r="D54" s="34"/>
@@ -6942,18 +6951,15 @@
       <c r="BL54" s="35"/>
     </row>
     <row r="55" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="68"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="71"/>
+      <c r="B55" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="66"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="58"/>
+      <c r="F55" s="58"/>
       <c r="G55" s="14"/>
-      <c r="H55" s="14" t="str">
-        <f t="shared" ref="H55:H56" si="8">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
-      </c>
+      <c r="H55" s="14"/>
       <c r="I55" s="35"/>
       <c r="J55" s="35"/>
       <c r="K55" s="35"/>
@@ -7012,25 +7018,17 @@
       <c r="BL55" s="35"/>
     </row>
     <row r="56" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="75" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="34">
-        <v>0.35</v>
-      </c>
-      <c r="E56" s="58">
-        <v>44156</v>
-      </c>
-      <c r="F56" s="58">
-        <v>44159</v>
-      </c>
+      <c r="B56" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="68"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="71"/>
       <c r="G56" s="14"/>
-      <c r="H56" s="14">
-        <f t="shared" si="8"/>
-        <v>4</v>
+      <c r="H56" s="14" t="str">
+        <f t="shared" ref="H56:H57" si="8">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
       </c>
       <c r="I56" s="35"/>
       <c r="J56" s="35"/>
@@ -7091,14 +7089,25 @@
     </row>
     <row r="57" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="75" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="66"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
+        <v>88</v>
+      </c>
+      <c r="C57" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="34">
+        <v>0.35</v>
+      </c>
+      <c r="E57" s="58">
+        <v>44156</v>
+      </c>
+      <c r="F57" s="58">
+        <v>44159</v>
+      </c>
       <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
+      <c r="H57" s="14">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
       <c r="I57" s="35"/>
       <c r="J57" s="35"/>
       <c r="K57" s="35"/>
@@ -7158,7 +7167,7 @@
     </row>
     <row r="58" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="75" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C58" s="66"/>
       <c r="D58" s="34"/>
@@ -7223,8 +7232,75 @@
       <c r="BK58" s="35"/>
       <c r="BL58" s="35"/>
     </row>
-    <row r="59" spans="2:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E59"/>
+    <row r="59" spans="2:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="66"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
+      <c r="P59" s="35"/>
+      <c r="Q59" s="35"/>
+      <c r="R59" s="35"/>
+      <c r="S59" s="35"/>
+      <c r="T59" s="35"/>
+      <c r="U59" s="35"/>
+      <c r="V59" s="35"/>
+      <c r="W59" s="35"/>
+      <c r="X59" s="35"/>
+      <c r="Y59" s="35"/>
+      <c r="Z59" s="35"/>
+      <c r="AA59" s="35"/>
+      <c r="AB59" s="35"/>
+      <c r="AC59" s="35"/>
+      <c r="AD59" s="35"/>
+      <c r="AE59" s="35"/>
+      <c r="AF59" s="35"/>
+      <c r="AG59" s="35"/>
+      <c r="AH59" s="35"/>
+      <c r="AI59" s="35"/>
+      <c r="AJ59" s="35"/>
+      <c r="AK59" s="35"/>
+      <c r="AL59" s="35"/>
+      <c r="AM59" s="35"/>
+      <c r="AN59" s="35"/>
+      <c r="AO59" s="35"/>
+      <c r="AP59" s="35"/>
+      <c r="AQ59" s="35"/>
+      <c r="AR59" s="35"/>
+      <c r="AS59" s="35"/>
+      <c r="AT59" s="35"/>
+      <c r="AU59" s="35"/>
+      <c r="AV59" s="35"/>
+      <c r="AW59" s="35"/>
+      <c r="AX59" s="35"/>
+      <c r="AY59" s="35"/>
+      <c r="AZ59" s="35"/>
+      <c r="BA59" s="35"/>
+      <c r="BB59" s="35"/>
+      <c r="BC59" s="35"/>
+      <c r="BD59" s="35"/>
+      <c r="BE59" s="35"/>
+      <c r="BF59" s="35"/>
+      <c r="BG59" s="35"/>
+      <c r="BH59" s="35"/>
+      <c r="BI59" s="35"/>
+      <c r="BJ59" s="35"/>
+      <c r="BK59" s="35"/>
+      <c r="BL59" s="35"/>
+    </row>
+    <row r="60" spans="2:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E60"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -7241,8 +7317,8 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D29 D47 D7:D14 D17:D18 D23:D26 D20:D21">
-    <cfRule type="dataBar" priority="182">
+  <conditionalFormatting sqref="D48 D29 D7:D14 D17:D18 D23:D26 D20:D21">
+    <cfRule type="dataBar" priority="183">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7255,21 +7331,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47 I29:BL29 I5:BL14 I17:BL18 I23:BL26 I20:BL21">
-    <cfRule type="expression" dxfId="104" priority="201">
+  <conditionalFormatting sqref="I48:BL48 I29:BL29 I5:BL14 I17:BL18 I23:BL26 I20:BL21 I32:BL32">
+    <cfRule type="expression" dxfId="104" priority="202">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47:BL47 I29:BL29 I7:BL14 I17:BL18 I23:BL26 I20:BL21">
-    <cfRule type="expression" dxfId="103" priority="195">
+  <conditionalFormatting sqref="I48:BL48 I29:BL29 I7:BL14 I17:BL18 I23:BL26 I20:BL21 I32:BL32">
+    <cfRule type="expression" dxfId="103" priority="196">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="197" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="dataBar" priority="165">
+    <cfRule type="dataBar" priority="166">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7283,20 +7359,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="101" priority="168">
+    <cfRule type="expression" dxfId="101" priority="169">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BL30">
-    <cfRule type="expression" dxfId="100" priority="166">
+    <cfRule type="expression" dxfId="100" priority="167">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="168" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="dataBar" priority="161">
+  <conditionalFormatting sqref="D38">
+    <cfRule type="dataBar" priority="162">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7309,21 +7385,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:BL37">
-    <cfRule type="expression" dxfId="98" priority="164">
+  <conditionalFormatting sqref="I38:BL38">
+    <cfRule type="expression" dxfId="98" priority="165">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:BL37">
-    <cfRule type="expression" dxfId="97" priority="162">
+  <conditionalFormatting sqref="I38:BL38">
+    <cfRule type="expression" dxfId="97" priority="163">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="164" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="dataBar" priority="157">
+  <conditionalFormatting sqref="D42">
+    <cfRule type="dataBar" priority="158">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7336,21 +7412,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41:BL41">
-    <cfRule type="expression" dxfId="95" priority="160">
+  <conditionalFormatting sqref="I42:BL42">
+    <cfRule type="expression" dxfId="95" priority="161">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41:BL41">
-    <cfRule type="expression" dxfId="94" priority="158">
+  <conditionalFormatting sqref="I42:BL42">
+    <cfRule type="expression" dxfId="94" priority="159">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="159" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="160" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="dataBar" priority="149">
+  <conditionalFormatting sqref="D34">
+    <cfRule type="dataBar" priority="150">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7363,21 +7439,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33:BL33">
-    <cfRule type="expression" dxfId="92" priority="152">
+  <conditionalFormatting sqref="I34:BL34">
+    <cfRule type="expression" dxfId="92" priority="153">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33:BL33">
-    <cfRule type="expression" dxfId="91" priority="150">
+  <conditionalFormatting sqref="I34:BL34">
+    <cfRule type="expression" dxfId="91" priority="151">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="152" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="dataBar" priority="145">
+  <conditionalFormatting sqref="D37">
+    <cfRule type="dataBar" priority="146">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7390,21 +7466,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="89" priority="148">
+  <conditionalFormatting sqref="I37:BL37">
+    <cfRule type="expression" dxfId="89" priority="149">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="88" priority="146">
+  <conditionalFormatting sqref="I37:BL37">
+    <cfRule type="expression" dxfId="88" priority="147">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="148" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="dataBar" priority="141">
+  <conditionalFormatting sqref="D39">
+    <cfRule type="dataBar" priority="142">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7417,21 +7493,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL38">
-    <cfRule type="expression" dxfId="86" priority="144">
+  <conditionalFormatting sqref="I39:BL39">
+    <cfRule type="expression" dxfId="86" priority="145">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:BL38">
-    <cfRule type="expression" dxfId="85" priority="142">
+  <conditionalFormatting sqref="I39:BL39">
+    <cfRule type="expression" dxfId="85" priority="143">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="144" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="dataBar" priority="137">
+  <conditionalFormatting sqref="D41">
+    <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7444,21 +7520,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:BL40">
-    <cfRule type="expression" dxfId="83" priority="140">
+  <conditionalFormatting sqref="I41:BL41">
+    <cfRule type="expression" dxfId="83" priority="141">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:BL40">
-    <cfRule type="expression" dxfId="82" priority="138">
+  <conditionalFormatting sqref="I41:BL41">
+    <cfRule type="expression" dxfId="82" priority="139">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="140" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="dataBar" priority="133">
+  <conditionalFormatting sqref="D43">
+    <cfRule type="dataBar" priority="134">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7471,21 +7547,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:BL42">
-    <cfRule type="expression" dxfId="80" priority="136">
+  <conditionalFormatting sqref="I43:BL43">
+    <cfRule type="expression" dxfId="80" priority="137">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:BL42">
-    <cfRule type="expression" dxfId="79" priority="134">
+  <conditionalFormatting sqref="I43:BL43">
+    <cfRule type="expression" dxfId="79" priority="135">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="136" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="dataBar" priority="129">
+  <conditionalFormatting sqref="D44">
+    <cfRule type="dataBar" priority="130">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7498,21 +7574,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:BL43">
-    <cfRule type="expression" dxfId="77" priority="132">
+  <conditionalFormatting sqref="I44:BL44">
+    <cfRule type="expression" dxfId="77" priority="133">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:BL43">
-    <cfRule type="expression" dxfId="76" priority="130">
+  <conditionalFormatting sqref="I44:BL44">
+    <cfRule type="expression" dxfId="76" priority="131">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="132" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="dataBar" priority="125">
+  <conditionalFormatting sqref="D45">
+    <cfRule type="dataBar" priority="126">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7525,21 +7601,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:BL44">
-    <cfRule type="expression" dxfId="74" priority="128">
+  <conditionalFormatting sqref="I45:BL45">
+    <cfRule type="expression" dxfId="74" priority="129">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:BL44">
-    <cfRule type="expression" dxfId="73" priority="126">
+  <conditionalFormatting sqref="I45:BL45">
+    <cfRule type="expression" dxfId="73" priority="127">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="128" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="dataBar" priority="113">
+  <conditionalFormatting sqref="D46">
+    <cfRule type="dataBar" priority="114">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7552,21 +7628,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45:BL45">
-    <cfRule type="expression" dxfId="71" priority="116">
+  <conditionalFormatting sqref="I46:BL46">
+    <cfRule type="expression" dxfId="71" priority="117">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45:BL45">
-    <cfRule type="expression" dxfId="70" priority="114">
+  <conditionalFormatting sqref="I46:BL46">
+    <cfRule type="expression" dxfId="70" priority="115">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="116" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="dataBar" priority="109">
+  <conditionalFormatting sqref="D47">
+    <cfRule type="dataBar" priority="110">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7579,21 +7655,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46:BL46">
-    <cfRule type="expression" dxfId="68" priority="112">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="68" priority="113">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46:BL46">
-    <cfRule type="expression" dxfId="67" priority="110">
+  <conditionalFormatting sqref="I47:BL47">
+    <cfRule type="expression" dxfId="67" priority="111">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="112" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="dataBar" priority="105">
+  <conditionalFormatting sqref="D49">
+    <cfRule type="dataBar" priority="106">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7606,21 +7682,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:BL48">
-    <cfRule type="expression" dxfId="65" priority="108">
+  <conditionalFormatting sqref="I49:BL49">
+    <cfRule type="expression" dxfId="65" priority="109">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:BL48">
-    <cfRule type="expression" dxfId="64" priority="106">
+  <conditionalFormatting sqref="I49:BL49">
+    <cfRule type="expression" dxfId="64" priority="107">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="108" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="dataBar" priority="97">
+    <cfRule type="dataBar" priority="98">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7634,20 +7710,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BL31">
-    <cfRule type="expression" dxfId="62" priority="100">
+    <cfRule type="expression" dxfId="62" priority="101">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BL31">
-    <cfRule type="expression" dxfId="61" priority="98">
+    <cfRule type="expression" dxfId="61" priority="99">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="100" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="dataBar" priority="93">
+  <conditionalFormatting sqref="D50">
+    <cfRule type="dataBar" priority="94">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7660,21 +7736,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49:BL49">
-    <cfRule type="expression" dxfId="59" priority="96">
+  <conditionalFormatting sqref="I50:BL50">
+    <cfRule type="expression" dxfId="59" priority="97">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49:BL49">
-    <cfRule type="expression" dxfId="58" priority="94">
+  <conditionalFormatting sqref="I50:BL50">
+    <cfRule type="expression" dxfId="58" priority="95">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="96" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="dataBar" priority="89">
+  <conditionalFormatting sqref="D40">
+    <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7687,21 +7763,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:BL39">
-    <cfRule type="expression" dxfId="56" priority="92">
+  <conditionalFormatting sqref="I40:BL40">
+    <cfRule type="expression" dxfId="56" priority="93">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39:BL39">
-    <cfRule type="expression" dxfId="55" priority="90">
+  <conditionalFormatting sqref="I40:BL40">
+    <cfRule type="expression" dxfId="55" priority="91">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="92" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="dataBar" priority="81">
+    <cfRule type="dataBar" priority="82">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7715,20 +7791,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BL28">
-    <cfRule type="expression" dxfId="53" priority="84">
+    <cfRule type="expression" dxfId="53" priority="85">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BL28">
-    <cfRule type="expression" dxfId="52" priority="82">
+    <cfRule type="expression" dxfId="52" priority="83">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="84" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="dataBar" priority="77">
+    <cfRule type="dataBar" priority="78">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7742,20 +7818,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BL15">
-    <cfRule type="expression" dxfId="50" priority="80">
+    <cfRule type="expression" dxfId="50" priority="81">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BL15">
-    <cfRule type="expression" dxfId="49" priority="78">
+    <cfRule type="expression" dxfId="49" priority="79">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="80" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="dataBar" priority="73">
+    <cfRule type="dataBar" priority="74">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7769,20 +7845,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BL16">
-    <cfRule type="expression" dxfId="47" priority="76">
+    <cfRule type="expression" dxfId="47" priority="77">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BL16">
-    <cfRule type="expression" dxfId="46" priority="74">
+    <cfRule type="expression" dxfId="46" priority="75">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="76" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="dataBar" priority="69">
+    <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7796,20 +7872,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:BL27">
-    <cfRule type="expression" dxfId="44" priority="72">
+    <cfRule type="expression" dxfId="44" priority="73">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:BL27">
-    <cfRule type="expression" dxfId="43" priority="70">
+    <cfRule type="expression" dxfId="43" priority="71">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="72" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="dataBar" priority="65">
+  <conditionalFormatting sqref="D35">
+    <cfRule type="dataBar" priority="66">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7822,21 +7898,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34:BL34">
-    <cfRule type="expression" dxfId="41" priority="68">
+  <conditionalFormatting sqref="I35:BL35">
+    <cfRule type="expression" dxfId="41" priority="69">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34:BL34">
-    <cfRule type="expression" dxfId="40" priority="66">
+  <conditionalFormatting sqref="I35:BL35">
+    <cfRule type="expression" dxfId="40" priority="67">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="68" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="dataBar" priority="57">
+  <conditionalFormatting sqref="D36">
+    <cfRule type="dataBar" priority="58">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7849,21 +7925,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:BL35">
-    <cfRule type="expression" dxfId="38" priority="60">
+  <conditionalFormatting sqref="I36:BL36">
+    <cfRule type="expression" dxfId="38" priority="61">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35:BL35">
-    <cfRule type="expression" dxfId="37" priority="58">
+  <conditionalFormatting sqref="I36:BL36">
+    <cfRule type="expression" dxfId="37" priority="59">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="60" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7877,20 +7953,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:BL22">
-    <cfRule type="expression" dxfId="35" priority="52">
+    <cfRule type="expression" dxfId="35" priority="53">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:BL22">
-    <cfRule type="expression" dxfId="34" priority="50">
+    <cfRule type="expression" dxfId="34" priority="51">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="52" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="dataBar" priority="45">
+  <conditionalFormatting sqref="D53">
+    <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7903,21 +7979,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52:BL52">
-    <cfRule type="expression" dxfId="32" priority="48">
+  <conditionalFormatting sqref="I53:BL53">
+    <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52:BL52">
-    <cfRule type="expression" dxfId="31" priority="46">
+  <conditionalFormatting sqref="I53:BL53">
+    <cfRule type="expression" dxfId="31" priority="47">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="48" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="dataBar" priority="41">
+  <conditionalFormatting sqref="D51">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7930,21 +8006,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50:BL50">
-    <cfRule type="expression" dxfId="29" priority="44">
+  <conditionalFormatting sqref="I51:BL51">
+    <cfRule type="expression" dxfId="29" priority="45">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50:BL50">
-    <cfRule type="expression" dxfId="28" priority="42">
+  <conditionalFormatting sqref="I51:BL51">
+    <cfRule type="expression" dxfId="28" priority="43">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="44" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="dataBar" priority="37">
+  <conditionalFormatting sqref="D52">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7957,21 +8033,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BL51">
-    <cfRule type="expression" dxfId="26" priority="40">
+  <conditionalFormatting sqref="I52:BL52">
+    <cfRule type="expression" dxfId="26" priority="41">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BL51">
-    <cfRule type="expression" dxfId="25" priority="38">
+  <conditionalFormatting sqref="I52:BL52">
+    <cfRule type="expression" dxfId="25" priority="39">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="40" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="dataBar" priority="33">
+  <conditionalFormatting sqref="D54">
+    <cfRule type="dataBar" priority="34">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7984,21 +8060,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL53">
-    <cfRule type="expression" dxfId="23" priority="36">
+  <conditionalFormatting sqref="I54:BL54">
+    <cfRule type="expression" dxfId="23" priority="37">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53:BL53">
-    <cfRule type="expression" dxfId="22" priority="34">
+  <conditionalFormatting sqref="I54:BL54">
+    <cfRule type="expression" dxfId="22" priority="35">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="dataBar" priority="29">
+  <conditionalFormatting sqref="D55">
+    <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8011,21 +8087,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I54:BL54">
-    <cfRule type="expression" dxfId="20" priority="32">
+  <conditionalFormatting sqref="I55:BL55">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I54:BL54">
-    <cfRule type="expression" dxfId="19" priority="30">
+  <conditionalFormatting sqref="I55:BL55">
+    <cfRule type="expression" dxfId="19" priority="31">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="32" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="dataBar" priority="25">
+  <conditionalFormatting sqref="D33">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8038,21 +8114,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL32">
-    <cfRule type="expression" dxfId="17" priority="28">
+  <conditionalFormatting sqref="I33:BL33">
+    <cfRule type="expression" dxfId="17" priority="29">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL32">
-    <cfRule type="expression" dxfId="16" priority="26">
+  <conditionalFormatting sqref="I33:BL33">
+    <cfRule type="expression" dxfId="16" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="28" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="dataBar" priority="21">
+  <conditionalFormatting sqref="D58">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8065,21 +8141,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:BL57">
-    <cfRule type="expression" dxfId="14" priority="24">
+  <conditionalFormatting sqref="I58:BL58">
+    <cfRule type="expression" dxfId="14" priority="25">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:BL57">
-    <cfRule type="expression" dxfId="13" priority="22">
+  <conditionalFormatting sqref="I58:BL58">
+    <cfRule type="expression" dxfId="13" priority="23">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="D56">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8092,21 +8168,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I55:BL55">
-    <cfRule type="expression" dxfId="11" priority="20">
+  <conditionalFormatting sqref="I56:BL56">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I55:BL55">
-    <cfRule type="expression" dxfId="10" priority="18">
+  <conditionalFormatting sqref="I56:BL56">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="20" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="D57">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8119,21 +8195,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL56">
-    <cfRule type="expression" dxfId="8" priority="16">
+  <conditionalFormatting sqref="I57:BL57">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:BL56">
-    <cfRule type="expression" dxfId="7" priority="14">
+  <conditionalFormatting sqref="I57:BL57">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="16" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="D59">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8146,21 +8222,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I58:BL58">
-    <cfRule type="expression" dxfId="5" priority="12">
+  <conditionalFormatting sqref="I59:BL59">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I58:BL58">
-    <cfRule type="expression" dxfId="4" priority="10">
+  <conditionalFormatting sqref="I59:BL59">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="12" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8174,16 +8250,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:BL19">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:BL19">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9CB3533F-9C4E-4000-BD74-A12298E78DEE}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -8213,7 +8303,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D29 D47 D7:D14 D17:D18 D23:D26 D20:D21</xm:sqref>
+          <xm:sqref>D48 D29 D7:D14 D17:D18 D23:D26 D20:D21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DEAB3775-453E-44CD-AB87-381933DECCDE}">
@@ -8243,7 +8333,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D37</xm:sqref>
+          <xm:sqref>D38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0096AF1A-393A-435C-8015-41D0DD370232}">
@@ -8258,7 +8348,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D41</xm:sqref>
+          <xm:sqref>D42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D4B26597-A923-4FC1-BDC5-A4D6F94E588D}">
@@ -8273,7 +8363,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D33</xm:sqref>
+          <xm:sqref>D34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2D9320E5-A90E-437D-95B7-E01E17503720}">
@@ -8288,7 +8378,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36</xm:sqref>
+          <xm:sqref>D37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{865C26A2-5F9B-4F2A-8497-BB5408076D73}">
@@ -8303,7 +8393,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D38</xm:sqref>
+          <xm:sqref>D39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4E847273-086C-4AA5-859E-6BF82F44FA57}">
@@ -8318,7 +8408,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D40</xm:sqref>
+          <xm:sqref>D41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FA2124C7-6797-44E6-8FD0-5B4542DBAA0C}">
@@ -8333,7 +8423,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D42</xm:sqref>
+          <xm:sqref>D43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{746A8A69-4303-484A-9428-BB46CDB16B19}">
@@ -8348,7 +8438,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D43</xm:sqref>
+          <xm:sqref>D44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5B84A7E2-E9E6-4BF2-B658-15D81FC470AE}">
@@ -8363,7 +8453,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D44</xm:sqref>
+          <xm:sqref>D45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D712486D-7533-424A-A845-4D223E96E211}">
@@ -8378,7 +8468,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D45</xm:sqref>
+          <xm:sqref>D46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B8D883F3-4418-4D7D-AF20-AD12CE96228A}">
@@ -8393,7 +8483,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D46</xm:sqref>
+          <xm:sqref>D47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{11B7A088-D8C3-40EB-8C27-1589CB10CFF4}">
@@ -8408,7 +8498,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D48</xm:sqref>
+          <xm:sqref>D49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{485CF41D-A6CA-4084-9D69-B8EDBA33F4BC}">
@@ -8438,7 +8528,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D49</xm:sqref>
+          <xm:sqref>D50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E62BDA41-A23E-4974-8AA5-16C1DA3F8E3F}">
@@ -8453,7 +8543,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D39</xm:sqref>
+          <xm:sqref>D40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FBF254AF-B480-422F-B5BE-2DAAD93F6F2A}">
@@ -8528,7 +8618,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34</xm:sqref>
+          <xm:sqref>D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0DD4499A-6C6E-44BD-9395-A72B26BB1533}">
@@ -8543,7 +8633,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35</xm:sqref>
+          <xm:sqref>D36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BBE71B1F-953F-4484-968A-62C8A2B711A6}">
@@ -8573,7 +8663,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D52</xm:sqref>
+          <xm:sqref>D53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{24113A02-1DBE-4064-9FC4-A65D86479F5A}">
@@ -8588,7 +8678,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D50</xm:sqref>
+          <xm:sqref>D51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1FE56A3A-A40B-46CB-8493-F121AFEF59C1}">
@@ -8603,7 +8693,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D51</xm:sqref>
+          <xm:sqref>D52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{10A6CA6A-D043-41E9-9CBD-6A680E0244A8}">
@@ -8618,7 +8708,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D53</xm:sqref>
+          <xm:sqref>D54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8CB5E189-86CB-4E67-8EB6-FB3FC8ABF181}">
@@ -8633,7 +8723,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D54</xm:sqref>
+          <xm:sqref>D55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7649434C-FFDA-47B7-B479-23E477DFB6E6}">
@@ -8648,7 +8738,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F083EF58-7FA3-4ADC-A83C-B309605218D3}">
@@ -8663,7 +8753,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D57</xm:sqref>
+          <xm:sqref>D58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CAB61D51-B9A4-4432-B966-CFC42510F8F6}">
@@ -8678,7 +8768,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D55</xm:sqref>
+          <xm:sqref>D56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5BC19FE3-5612-45A0-AC9B-98885C2CBB77}">
@@ -8693,7 +8783,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D56</xm:sqref>
+          <xm:sqref>D57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{035C63EA-A9B5-4A07-9B62-9F4F83C063D1}">
@@ -8708,7 +8798,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D58</xm:sqref>
+          <xm:sqref>D59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A0BC3692-3B2D-4B85-A1DC-054E03ECC8E3}">
@@ -8724,6 +8814,21 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>D19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9CB3533F-9C4E-4000-BD74-A12298E78DEE}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>